<commit_message>
Patching and test plan done.
</commit_message>
<xml_diff>
--- a/admin/writeups/Test Plan.xlsx
+++ b/admin/writeups/Test Plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\DGM\Y13 digital media\Juan Coetzee\admin\writeups\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\database\13DGM\admin\writeups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCED5A6-C0D3-4AB9-89C3-D2AA39694099}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7F67F1-EF7B-479C-8EA9-8D11D83FAEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{53C69F9E-5BA0-47ED-8C91-DB5D9436D550}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{53C69F9E-5BA0-47ED-8C91-DB5D9436D550}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="92">
   <si>
     <t>Test Plan</t>
-  </si>
-  <si>
-    <t>Test table for…….</t>
   </si>
   <si>
     <t>Test number</t>
@@ -225,7 +222,85 @@
     <t>The page has text clipping issue on multiple pages. Or layouts can change</t>
   </si>
   <si>
-    <t>To fix this I have decieded to reformat how some of the content is displayed. I  reformatted everything to a table.</t>
+    <t>To fix this I have decieded to reformat how some of the content is displayed. I  reformatted everything to a table for the lessons page. This allowed me to get images next to text in all screen sizes. For the micro:bits page the divs that containted the content were split into two. This allowed the content to always be seprated</t>
+  </si>
+  <si>
+    <t>All content in the correct area</t>
+  </si>
+  <si>
+    <t>The content should be in the correct are on the intended screen size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On the micro:bit page the header that says "Micro:bits specs" does not line up in the center. </t>
+  </si>
+  <si>
+    <t>I just need to lower a margin of the text above it. As this just touched the header</t>
+  </si>
+  <si>
+    <t>Quick list shrink correctly</t>
+  </si>
+  <si>
+    <t>All pages that have a quick list</t>
+  </si>
+  <si>
+    <t>This should hide the options on the quick list the more the page is shrunk, because shrinking text becomes harder to see</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All pages with headings </t>
+  </si>
+  <si>
+    <t>Swapping theme messing with headlines</t>
+  </si>
+  <si>
+    <t>The headline colours should change to fit the mode.</t>
+  </si>
+  <si>
+    <t>The headlines dissappear. Instead of changing colours</t>
+  </si>
+  <si>
+    <t>The would not hide and they would constanly move around</t>
+  </si>
+  <si>
+    <t>Overflow hidden was added to the quick list div</t>
+  </si>
+  <si>
+    <t>Just needed to rename the header to headline in the other themes stylesheet</t>
+  </si>
+  <si>
+    <t>Lessons content is bold</t>
+  </si>
+  <si>
+    <t>Lessons page only</t>
+  </si>
+  <si>
+    <t>The text would be unform and normal</t>
+  </si>
+  <si>
+    <t>The text in the table was bold without being to.</t>
+  </si>
+  <si>
+    <t>I added font-weight: normal; to each individual paragraph. My working theory is that putting text in a table automatically bolds the text.</t>
+  </si>
+  <si>
+    <t>All links to pages work</t>
+  </si>
+  <si>
+    <t>Every hyperlink on the website</t>
+  </si>
+  <si>
+    <t>By clicking on each hyperlink confirming where it takes you</t>
+  </si>
+  <si>
+    <t>All links should take you to the correct locations</t>
+  </si>
+  <si>
+    <t>The link between Mico:bits and About us didn't work</t>
+  </si>
+  <si>
+    <t>Added pathing between them.</t>
+  </si>
+  <si>
+    <t>Test table for The Micro:bits website</t>
   </si>
 </sst>
 </file>
@@ -263,7 +338,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -383,11 +458,85 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -433,6 +582,33 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -750,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9986A4B5-5129-4989-8F4A-4330BBD06915}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,13 +943,13 @@
     <col min="10" max="10" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="46.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="31.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>91</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -829,34 +1005,34 @@
     </row>
     <row r="3" spans="1:26" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -875,32 +1051,32 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" spans="1:26" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="10"/>
@@ -919,32 +1095,32 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5" spans="1:26" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="115.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="J5" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="K5" s="8"/>
       <c r="L5" s="11"/>
@@ -963,32 +1139,32 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" spans="1:26" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" ht="167.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="I6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="J6" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K6" s="8"/>
       <c r="L6" s="12"/>
@@ -1007,32 +1183,32 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" spans="1:26" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="160.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="I7" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K7" s="8"/>
       <c r="L7" s="13"/>
@@ -1051,32 +1227,32 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" spans="1:26" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="I8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="J8" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="K8" s="8"/>
       <c r="L8" s="13"/>
@@ -1095,32 +1271,32 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" spans="1:26" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="I9" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="I9" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="J9" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K9" s="8"/>
       <c r="L9" s="13"/>
@@ -1139,32 +1315,32 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:26" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="I10" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="I10" s="5" t="s">
-        <v>66</v>
-      </c>
       <c r="J10" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K10" s="8"/>
       <c r="L10" s="13"/>
@@ -1183,32 +1359,32 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" spans="1:26" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>8</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="I11" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="I11" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="J11" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K11" s="8"/>
       <c r="L11" s="13"/>
@@ -1232,27 +1408,27 @@
         <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H12" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="I12" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="J12" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K12" s="8"/>
       <c r="L12" s="13"/>
@@ -1271,32 +1447,32 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13" spans="1:26" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>10</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="I13" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="I13" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="J13" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K13" s="8"/>
       <c r="L13" s="13"/>
@@ -1315,17 +1491,33 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+    <row r="14" spans="1:26" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>11</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
+      <c r="G14" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="K14" s="8"/>
       <c r="L14" s="13"/>
       <c r="M14" s="11"/>
@@ -1343,17 +1535,33 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+    <row r="15" spans="1:26" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>12</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
+      <c r="G15" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="K15" s="8"/>
       <c r="L15" s="13"/>
       <c r="M15" s="11"/>
@@ -1371,17 +1579,33 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+    <row r="16" spans="1:26" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="16">
+        <v>13</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
+      <c r="G16" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="K16" s="8"/>
       <c r="L16" s="13"/>
       <c r="M16" s="11"/>
@@ -1399,18 +1623,34 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="8"/>
+    <row r="17" spans="1:26" ht="108" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="22">
+        <v>14</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="I17" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="J17" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="K17" s="19"/>
       <c r="L17" s="13"/>
       <c r="M17" s="11"/>
       <c r="N17" s="9"/>
@@ -1427,18 +1667,34 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="8"/>
+    <row r="18" spans="1:26" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="23">
+        <v>15</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="H18" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="I18" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J18" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="K18" s="11"/>
       <c r="L18" s="13"/>
       <c r="M18" s="11"/>
       <c r="N18" s="9"/>
@@ -1456,17 +1712,16 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="8"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="11"/>
       <c r="L19" s="13"/>
       <c r="M19" s="11"/>
       <c r="N19" s="9"/>
@@ -1484,17 +1739,17 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="8"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="11"/>
       <c r="L20" s="13"/>
       <c r="M20" s="11"/>
       <c r="N20" s="9"/>
@@ -1512,18 +1767,18 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="7"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="17"/>
       <c r="M21" s="7"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
@@ -1540,18 +1795,18 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="9"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
@@ -1568,18 +1823,18 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="9"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
@@ -1596,18 +1851,18 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="9"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
@@ -1624,18 +1879,18 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="9"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
@@ -1652,18 +1907,18 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="9"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
@@ -1680,17 +1935,17 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="1"/>
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="7"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>

</xml_diff>